<commit_message>
todas las opciones funcionando ok, 1er etapa de pruebas y correcion de errores
</commit_message>
<xml_diff>
--- a/php/admin/cobros/3_caja_final.xlsx
+++ b/php/admin/cobros/3_caja_final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -27,7 +27,7 @@
     <t>GUARDO registro anterior sumado</t>
   </si>
   <si>
-    <t>ft_actual    SUMA LAS DOS ANTERIORES ES EL SALDO ACTUAL restando la extraccion</t>
+    <t xml:space="preserve">ft_actual    SUMA LAS DOS ANTERIORES ES EL SALDO ACTUAL </t>
   </si>
   <si>
     <t>EXTRACCION  ft</t>
@@ -96,7 +96,10 @@
     <t>pago movil</t>
   </si>
   <si>
-    <t>extraccion</t>
+    <t>dep ft/mp movil</t>
+  </si>
+  <si>
+    <t>extraccion ft/mp</t>
   </si>
   <si>
     <t>Deposito</t>
@@ -110,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +130,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -158,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -172,47 +182,41 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,26 +528,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="16" width="34.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="135.75">
@@ -565,16 +569,16 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -609,22 +613,22 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -650,23 +654,23 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>1000</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
@@ -684,21 +688,21 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>2000</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>1000</v>
       </c>
       <c r="D4" s="4">
         <v>3000</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
@@ -716,25 +720,31 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>7000</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>3000</v>
       </c>
       <c r="D5" s="4">
         <v>10000</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="8">
+        <v>4500</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4500</v>
+      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -748,25 +758,31 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>2500</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>10000</v>
       </c>
       <c r="D6" s="4">
         <v>12500</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8">
+        <v>6100</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4500</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10600</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -780,25 +796,31 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>8500</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>12500</v>
       </c>
       <c r="D7" s="4">
         <v>21000</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10600</v>
+      </c>
+      <c r="I7" s="2">
+        <v>13600</v>
+      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -812,19 +834,25 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
       <c r="E8" s="4">
         <v>21000</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="8">
+        <v>5000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>13600</v>
+      </c>
+      <c r="I8" s="2">
+        <v>18600</v>
+      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
@@ -842,20 +870,28 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="8">
+        <v>30400</v>
+      </c>
+      <c r="H9" s="2">
+        <v>18600</v>
+      </c>
+      <c r="I9" s="2">
+        <v>22000</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -868,25 +904,27 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>9200</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>0</v>
       </c>
       <c r="D10" s="4">
         <v>9200</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <v>22000</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3" t="s">
-        <v>25</v>
+      <c r="M10" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -900,26 +938,24 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>9200</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>9200</v>
       </c>
       <c r="D11" s="4">
         <v>18400</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -932,21 +968,21 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4">
         <v>20000</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -957,312 +993,280 @@
       <c r="T12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>20000</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="5">
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="11">
-        <v>4500</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
-        <v>4500</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="5">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="11">
-        <v>6100</v>
-      </c>
-      <c r="H15" s="12">
-        <v>4500</v>
-      </c>
-      <c r="I15" s="12">
-        <v>10600</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="5">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="11">
-        <v>3000</v>
-      </c>
-      <c r="H16" s="12">
-        <v>10600</v>
-      </c>
-      <c r="I16" s="12">
-        <v>13600</v>
-      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="5">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="11">
-        <v>5000</v>
-      </c>
-      <c r="H17" s="12">
-        <v>13600</v>
-      </c>
-      <c r="I17" s="12">
-        <v>18600</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="5">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="11">
-        <v>30400</v>
-      </c>
-      <c r="H18" s="12">
-        <v>18600</v>
-      </c>
-      <c r="I18" s="12">
-        <v>22000</v>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="5">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="12">
-        <v>22000</v>
-      </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="5">
+      <c r="J19" s="10"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="11">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="8">
         <v>0</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="5">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="13">
-      <c r="A23" s="7">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="11">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>